<commit_message>
adicionando os testes negativos
</commit_message>
<xml_diff>
--- a/target/TestDta/BuscarProduto.xlsx
+++ b/target/TestDta/BuscarProduto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0C3560E1-817C-4FC1-8487-7841165BEAC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3EB2D3C7-B6E5-4497-A795-D9BE5C7D184C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20490" windowHeight="11820" xr2:uid="{3811DB8B-1056-40F0-864D-B037B3637F44}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20520" windowHeight="11820" xr2:uid="{3811DB8B-1056-40F0-864D-B037B3637F44}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>HP ZBOOK 17 G2 MOBILE WORKSTATION</t>
   </si>
@@ -42,12 +42,16 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -453,11 +457,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="0.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="47.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="0.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -485,7 +489,9 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">

</xml_diff>